<commit_message>
Updated Codes for IHE NA connectathon
</commit_message>
<xml_diff>
--- a/CodesForSDCinMHD.xlsx
+++ b/CodesForSDCinMHD.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6900"/>
   </bookViews>
   <sheets>
     <sheet name="SDCRadiology" sheetId="1" r:id="rId1"/>
@@ -708,7 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -757,9 +757,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -796,6 +793,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1114,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1133,7 +1139,7 @@
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1244,7 +1250,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+      <c r="A14" s="31" t="s">
         <v>30</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -1273,13 +1279,13 @@
       <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E15" s="18" t="s">
+      <c r="D15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="33" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="34" t="s">
         <v>42</v>
       </c>
       <c r="G15" s="15"/>
@@ -1294,10 +1300,10 @@
       <c r="D16" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="20" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="15" t="s">
@@ -1352,7 +1358,7 @@
       <c r="D19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="18" t="s">
+      <c r="E19" s="33" t="s">
         <v>18</v>
       </c>
       <c r="F19" s="6" t="s">
@@ -1367,10 +1373,14 @@
     <hyperlink ref="D16" r:id="rId3" display="http://hl7.org/fhir/valueset-formatcodes.html"/>
     <hyperlink ref="F16" r:id="rId4"/>
     <hyperlink ref="B1" r:id="rId5"/>
+    <hyperlink ref="E15" r:id="rId6"/>
+    <hyperlink ref="F15" r:id="rId7"/>
+    <hyperlink ref="E16" r:id="rId8"/>
+    <hyperlink ref="E19" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
-  <legacyDrawing r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
+  <legacyDrawing r:id="rId11"/>
 </worksheet>
 </file>
 
@@ -1379,7 +1389,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1407,7 @@
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1507,78 +1517,78 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+    <row r="14" spans="1:7" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="22" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
       <c r="B15" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="25" t="s">
+      <c r="D15" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="25" t="s">
         <v>42</v>
       </c>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" s="22" customFormat="1" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="21" customFormat="1" ht="87.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="20" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="24" t="s">
         <v>32</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -1586,17 +1596,17 @@
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="2:7" s="22" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" s="21" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="30" t="s">
         <v>33</v>
       </c>
       <c r="F18" s="9" t="s">
@@ -1606,7 +1616,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:7" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
@@ -1616,7 +1626,7 @@
       <c r="D19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="24" t="s">
         <v>18</v>
       </c>
       <c r="F19" s="6" t="s">
@@ -1642,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1661,7 +1671,7 @@
       <c r="A1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1771,78 +1781,78 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
+    <row r="14" spans="1:7" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="23" t="s">
+      <c r="D14" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="E14" s="23" t="s">
+      <c r="E14" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="G14" s="23" t="s">
+      <c r="G14" s="22" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>1</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="25" t="s">
+      <c r="E15" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="26" t="s">
+      <c r="F15" s="25" t="s">
         <v>42</v>
       </c>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="1:7" s="22" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" s="21" customFormat="1" ht="78.75" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>2</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="20" t="s">
         <v>15</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="25" t="s">
+      <c r="E17" s="24" t="s">
         <v>32</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -1850,17 +1860,17 @@
       </c>
       <c r="G17" s="6"/>
     </row>
-    <row r="18" spans="2:7" s="22" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7" s="21" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="s">
         <v>4</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="30" t="s">
         <v>33</v>
       </c>
       <c r="F18" s="9" t="s">
@@ -1870,7 +1880,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="2:7" s="22" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" s="21" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="B19" s="6" t="s">
         <v>5</v>
       </c>
@@ -1880,7 +1890,7 @@
       <c r="D19" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="25" t="s">
+      <c r="E19" s="24" t="s">
         <v>18</v>
       </c>
       <c r="F19" s="6" t="s">

</xml_diff>